<commit_message>
add chi 2 to methods list
</commit_message>
<xml_diff>
--- a/data/methods_dictionary.xlsx
+++ b/data/methods_dictionary.xlsx
@@ -1,40 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectqutedu-my.sharepoint.com/personal/whitenm_qut_edu_au/Documents/Git projects/stats_section/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectqutedu-my.sharepoint.com/personal/whitenm_qut_edu_au/Documents/Git projects/stats_section/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{187F6103-615A-47C5-BA3D-1C61B4FE5D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D7EC2704-2C22-4A93-8F49-129426E353A7}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{187F6103-615A-47C5-BA3D-1C61B4FE5D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D0F5402C-0B47-4F36-985E-67512D9BD8CB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6941413E-72A1-4783-89A4-EE179FBDE9B1}"/>
+    <workbookView xWindow="28800" yWindow="480" windowWidth="28800" windowHeight="12345" xr2:uid="{6941413E-72A1-4783-89A4-EE179FBDE9B1}"/>
   </bookViews>
   <sheets>
     <sheet name="stats_terms" sheetId="1" r:id="rId1"/>
     <sheet name="other" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="299">
   <si>
     <t>update</t>
   </si>
@@ -928,6 +920,9 @@
   </si>
   <si>
     <t>v shaped</t>
+  </si>
+  <si>
+    <t>chi 2</t>
   </si>
 </sst>
 </file>
@@ -1283,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85770F85-B2D3-4508-9B12-71AB5E6420BB}">
-  <dimension ref="A1:H145"/>
+  <dimension ref="A1:H146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,16 +1482,16 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="A25" t="s">
+        <v>298</v>
+      </c>
+      <c r="B25" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>134</v>
@@ -1504,159 +1499,159 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>280</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>177</v>
-      </c>
-      <c r="B28" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B29" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
       <c r="B30" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>203</v>
+      </c>
+      <c r="B31" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>235</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>236</v>
-      </c>
-      <c r="B33" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>236</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>237</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>175</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>20</v>
+        <v>284</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>202</v>
+        <v>62</v>
       </c>
       <c r="B39" t="s">
-        <v>202</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>202</v>
+      </c>
+      <c r="B40" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>201</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>126</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>105</v>
-      </c>
-      <c r="B44" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>198</v>
+        <v>105</v>
       </c>
       <c r="B45" t="s">
-        <v>197</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B46" t="s">
         <v>197</v>
@@ -1664,162 +1659,162 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>77</v>
+        <v>197</v>
       </c>
       <c r="B47" t="s">
-        <v>78</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B48" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>178</v>
+        <v>58</v>
       </c>
       <c r="B49" t="s">
-        <v>222</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>239</v>
+        <v>178</v>
       </c>
       <c r="B50" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>239</v>
       </c>
       <c r="B51" t="s">
-        <v>22</v>
+        <v>239</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>182</v>
+        <v>64</v>
       </c>
       <c r="B52" t="s">
-        <v>226</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="B53" t="s">
-        <v>194</v>
+        <v>226</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B54" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>172</v>
+        <v>195</v>
       </c>
       <c r="B55" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B56" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>45</v>
+        <v>167</v>
       </c>
       <c r="B57" t="s">
-        <v>233</v>
+        <v>210</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>169</v>
+        <v>45</v>
       </c>
       <c r="B58" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B59" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="B60" t="s">
-        <v>23</v>
+        <v>216</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B61" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>35</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>67</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>85</v>
-      </c>
-      <c r="B66" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1832,378 +1827,378 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>180</v>
+        <v>85</v>
       </c>
       <c r="B68" t="s">
-        <v>224</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="B69" t="s">
-        <v>34</v>
+        <v>224</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>238</v>
+        <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>295</v>
+        <v>34</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>68</v>
+        <v>238</v>
       </c>
       <c r="B71" t="s">
-        <v>26</v>
+        <v>295</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>163</v>
+        <v>68</v>
       </c>
       <c r="B72" t="s">
-        <v>206</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="B73" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="B74" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B75" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>66</v>
+        <v>162</v>
       </c>
       <c r="B76" t="s">
-        <v>24</v>
+        <v>205</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B77" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>70</v>
+      </c>
+      <c r="B78" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>69</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>151</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>71</v>
-      </c>
-      <c r="B81" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B82" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B83" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B84" t="s">
-        <v>285</v>
+        <v>18</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>161</v>
+        <v>50</v>
       </c>
       <c r="B85" t="s">
-        <v>204</v>
+        <v>285</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>161</v>
+      </c>
+      <c r="B86" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>193</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B88" s="1" t="s">
         <v>232</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>44</v>
-      </c>
-      <c r="B88" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B89" t="s">
-        <v>286</v>
+        <v>218</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>47</v>
+      </c>
+      <c r="B90" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>48</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B93" s="1" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>49</v>
-      </c>
-      <c r="B93" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>49</v>
+      </c>
+      <c r="B94" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>166</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B95" t="s">
         <v>209</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>113</v>
-      </c>
-      <c r="B97" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="B98" t="s">
-        <v>289</v>
+        <v>114</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>281</v>
+        <v>51</v>
       </c>
       <c r="B99" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>37</v>
+        <v>281</v>
       </c>
       <c r="B100" t="s">
-        <v>3</v>
+        <v>290</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>115</v>
+        <v>37</v>
       </c>
       <c r="B101" t="s">
-        <v>116</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="B102" t="s">
-        <v>2</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>107</v>
+        <v>36</v>
       </c>
       <c r="B103" t="s">
-        <v>108</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B104" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="B105" t="s">
-        <v>291</v>
+        <v>110</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="B106" t="s">
-        <v>112</v>
+        <v>291</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="B107" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="B108" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>73</v>
+      </c>
+      <c r="B109" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>55</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B110" t="s">
         <v>292</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B112" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>196</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B113" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B114" s="1" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>87</v>
-      </c>
-      <c r="B114" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -2215,248 +2210,256 @@
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+      <c r="A116" t="s">
+        <v>87</v>
+      </c>
+      <c r="B116" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B117" s="1" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>164</v>
-      </c>
-      <c r="B117" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="B118" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="B119" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="B120" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>43</v>
+        <v>200</v>
       </c>
       <c r="B121" t="s">
-        <v>10</v>
+        <v>200</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
+        <v>43</v>
+      </c>
+      <c r="B122" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>190</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B123" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B124" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>124</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B125" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B126" s="1" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>184</v>
-      </c>
-      <c r="B126" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="B127" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="B128" t="s">
-        <v>293</v>
+        <v>211</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>282</v>
+        <v>52</v>
       </c>
       <c r="B129" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>38</v>
+        <v>282</v>
       </c>
       <c r="B130" t="s">
-        <v>4</v>
+        <v>283</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="B131" t="s">
-        <v>81</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B132" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B133" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B134" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B135" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>297</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>296</v>
+        <v>86</v>
+      </c>
+      <c r="B136" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>74</v>
-      </c>
-      <c r="B137" t="s">
-        <v>32</v>
+        <v>297</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>187</v>
+        <v>74</v>
       </c>
       <c r="B138" t="s">
-        <v>231</v>
+        <v>32</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="B139" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>92</v>
+        <v>181</v>
       </c>
       <c r="B140" t="s">
-        <v>100</v>
+        <v>225</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B141" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B142" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B143" t="s">
-        <v>96</v>
-      </c>
-      <c r="H143" s="1"/>
+        <v>98</v>
+      </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="B144" t="s">
-        <v>9</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="H144" s="1"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>42</v>
+      </c>
+      <c r="B145" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>41</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B146" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B146">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B147">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2628,6 +2631,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005144375E58E94B4797547602088A153E" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2716c96d3b4f6e6de2e4e819fa088272">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a21de7b9-cad9-43f2-8459-9b1b4f9894e2" xmlns:ns4="d0ad2d52-4869-465d-a93a-001fa21a593d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb21f0a81310d37a2f3dadcff746745c" ns3:_="" ns4:_="">
     <xsd:import namespace="a21de7b9-cad9-43f2-8459-9b1b4f9894e2"/>
@@ -2850,22 +2868,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD1FD567-2A85-4F72-A210-3107A4B71641}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47F11217-CA31-44E5-9155-3D53FF9AB52B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F34583C6-0E72-4AF2-A7BB-BC9CA2650495}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2882,21 +2902,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47F11217-CA31-44E5-9155-3D53FF9AB52B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD1FD567-2A85-4F72-A210-3107A4B71641}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add common words missed
</commit_message>
<xml_diff>
--- a/data/methods_dictionary.xlsx
+++ b/data/methods_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectqutedu-my.sharepoint.com/personal/whitenm_qut_edu_au/Documents/Git projects/stats_section/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="403" documentId="8_{187F6103-615A-47C5-BA3D-1C61B4FE5D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4FEDA78F-2926-4B2A-9CB1-781E28C53409}"/>
+  <xr:revisionPtr revIDLastSave="423" documentId="8_{187F6103-615A-47C5-BA3D-1C61B4FE5D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BF1B7AD5-222C-4A4F-A673-1FE0EF913AA2}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="195" windowWidth="28800" windowHeight="15060" activeTab="1" xr2:uid="{6941413E-72A1-4783-89A4-EE179FBDE9B1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6941413E-72A1-4783-89A4-EE179FBDE9B1}"/>
   </bookViews>
   <sheets>
     <sheet name="hyphen_terms" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="363">
   <si>
     <t>update</t>
   </si>
@@ -1087,6 +1087,36 @@
   </si>
   <si>
     <t>wilcoxons</t>
+  </si>
+  <si>
+    <t>u statistic</t>
+  </si>
+  <si>
+    <t>u-statistic</t>
+  </si>
+  <si>
+    <t>u test</t>
+  </si>
+  <si>
+    <t>u-test</t>
+  </si>
+  <si>
+    <t>non normally</t>
+  </si>
+  <si>
+    <t>non-normally</t>
+  </si>
+  <si>
+    <t>homoskedastic</t>
+  </si>
+  <si>
+    <t>homoscedastic</t>
+  </si>
+  <si>
+    <t>homoskedasticity</t>
+  </si>
+  <si>
+    <t>homoscedasticity</t>
   </si>
 </sst>
 </file>
@@ -1442,10 +1472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85770F85-B2D3-4508-9B12-71AB5E6420BB}">
-  <dimension ref="A1:H133"/>
+  <dimension ref="A1:H136"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2143,383 +2173,407 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>113</v>
+        <v>357</v>
       </c>
       <c r="B87" t="s">
-        <v>114</v>
+        <v>358</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>291</v>
+        <v>113</v>
       </c>
       <c r="B88" t="s">
-        <v>292</v>
+        <v>114</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>51</v>
+        <v>291</v>
       </c>
       <c r="B89" t="s">
-        <v>277</v>
+        <v>292</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>269</v>
+        <v>51</v>
       </c>
       <c r="B90" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>37</v>
+        <v>269</v>
       </c>
       <c r="B91" t="s">
-        <v>3</v>
+        <v>278</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>115</v>
+        <v>37</v>
       </c>
       <c r="B92" t="s">
-        <v>116</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="B93" t="s">
-        <v>2</v>
+        <v>116</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>107</v>
+        <v>36</v>
       </c>
       <c r="B94" t="s">
-        <v>108</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B95" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="B96" t="s">
-        <v>279</v>
+        <v>110</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="B97" t="s">
-        <v>112</v>
+        <v>279</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="B98" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="B99" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>73</v>
+      </c>
+      <c r="B100" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>55</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B101" t="s">
         <v>280</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B104" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>87</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B105" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B106" s="1" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>164</v>
-      </c>
-      <c r="B106" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="B107" t="s">
-        <v>221</v>
+        <v>199</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="B108" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>43</v>
+        <v>175</v>
       </c>
       <c r="B109" t="s">
-        <v>10</v>
+        <v>211</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>301</v>
+        <v>43</v>
       </c>
       <c r="B110" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+      <c r="A111" t="s">
+        <v>301</v>
+      </c>
+      <c r="B111" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B112" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>124</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B113" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B114" s="1" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>183</v>
-      </c>
-      <c r="B114" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="B115" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="B116" t="s">
-        <v>281</v>
+        <v>203</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>270</v>
+        <v>52</v>
       </c>
       <c r="B117" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>38</v>
+        <v>270</v>
       </c>
       <c r="B118" t="s">
-        <v>4</v>
+        <v>271</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="B119" t="s">
-        <v>81</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B120" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B121" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B122" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B123" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>285</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>284</v>
+        <v>86</v>
+      </c>
+      <c r="B124" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>74</v>
+        <v>353</v>
       </c>
       <c r="B125" t="s">
-        <v>32</v>
+        <v>354</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>186</v>
+        <v>355</v>
       </c>
       <c r="B126" t="s">
-        <v>222</v>
-      </c>
-      <c r="H126" s="1"/>
+        <v>356</v>
+      </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>180</v>
-      </c>
-      <c r="B127" t="s">
-        <v>216</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="H127" s="1"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="B128" t="s">
-        <v>100</v>
+        <v>32</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>94</v>
+        <v>186</v>
       </c>
       <c r="B129" t="s">
-        <v>102</v>
+        <v>222</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="B130" t="s">
-        <v>98</v>
+        <v>216</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B131" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="B132" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>90</v>
+      </c>
+      <c r="B133" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>88</v>
+      </c>
+      <c r="B134" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>42</v>
+      </c>
+      <c r="B135" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>41</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B136" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B134">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B137">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2532,7 +2586,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2815,16 +2869,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8997BC0-CEB9-4923-B89B-89A2832FF20E}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2977,6 +3031,22 @@
       </c>
       <c r="B19" t="s">
         <v>195</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>359</v>
+      </c>
+      <c r="B20" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>361</v>
+      </c>
+      <c r="B21" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -2985,9 +3055,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3214,19 +3287,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47F11217-CA31-44E5-9155-3D53FF9AB52B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD1FD567-2A85-4F72-A210-3107A4B71641}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3251,9 +3320,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD1FD567-2A85-4F72-A210-3107A4B71641}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47F11217-CA31-44E5-9155-3D53FF9AB52B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>